<commit_message>
clean up tagging data templates
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
@@ -12,11 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="7035" windowHeight="1815"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="scale envelope labels" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$AI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AJ$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Fish #</t>
   </si>
@@ -142,16 +142,7 @@
     <t>Box</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>from Tank</t>
-  </si>
-  <si>
     <t>Tagger</t>
-  </si>
-  <si>
-    <t>Amt MS222(g)</t>
   </si>
   <si>
     <t>Date
@@ -179,15 +170,9 @@
     <t>scale evelope label</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>cut and paste to template</t>
   </si>
   <si>
-    <t>to tank</t>
-  </si>
-  <si>
     <t>anesthetic water temp</t>
   </si>
   <si>
@@ -204,6 +189,24 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>To Tank</t>
+  </si>
+  <si>
+    <t>From Tank</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Amt</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -365,11 +368,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,6 +451,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -790,13 +807,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,28 +826,29 @@
     <col min="7" max="7" width="11.140625" style="10" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="10" customWidth="1"/>
     <col min="11" max="12" width="4.42578125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="4.42578125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="46.85546875" style="10" customWidth="1"/>
     <col min="15" max="19" width="9.140625" style="10"/>
-    <col min="20" max="20" width="10.7109375" style="10" customWidth="1"/>
-    <col min="21" max="27" width="9.140625" style="10"/>
-    <col min="28" max="28" width="16.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.140625" style="10"/>
-    <col min="31" max="31" width="28.5703125" style="10" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="10"/>
-    <col min="33" max="33" width="23.5703125" style="11" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="10"/>
+    <col min="20" max="21" width="10.7109375" style="10" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" style="10" customWidth="1"/>
+    <col min="23" max="28" width="9.140625" style="10"/>
+    <col min="29" max="29" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="9.140625" style="10"/>
+    <col min="32" max="32" width="28.5703125" style="10" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" style="10"/>
+    <col min="34" max="34" width="23.5703125" style="11" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>2</v>
@@ -858,74 +876,77 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="AA1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="AB1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="18" t="s">
+      <c r="AC1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AG1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -970,9 +991,10 @@
       <c r="AQ2"/>
       <c r="AR2"/>
       <c r="AS2"/>
+      <c r="AT2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI1">
+  <autoFilter ref="A1:AJ1">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <sortState ref="A2:AG285">

</xml_diff>

<commit_message>
add precocity to cb tagging parser, fix loading gif
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7035" windowHeight="1815"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7035" windowHeight="1815"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="scale envelope labels" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Fish #</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Amt</t>
+  </si>
+  <si>
+    <t>Precocity (1/0)</t>
   </si>
 </sst>
 </file>
@@ -447,13 +450,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -807,13 +810,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,19 +831,20 @@
     <col min="11" max="12" width="4.42578125" style="10" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="46.85546875" style="10" customWidth="1"/>
-    <col min="15" max="19" width="9.140625" style="10"/>
-    <col min="20" max="21" width="10.7109375" style="10" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="10" customWidth="1"/>
-    <col min="23" max="28" width="9.140625" style="10"/>
-    <col min="29" max="29" width="16.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="9.140625" style="10"/>
-    <col min="32" max="32" width="28.5703125" style="10" customWidth="1"/>
-    <col min="33" max="33" width="9.140625" style="10"/>
-    <col min="34" max="34" width="23.5703125" style="11" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="10"/>
+    <col min="15" max="15" width="27.42578125" style="10" customWidth="1"/>
+    <col min="16" max="20" width="9.140625" style="10"/>
+    <col min="21" max="22" width="10.7109375" style="10" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="10" customWidth="1"/>
+    <col min="24" max="29" width="9.140625" style="10"/>
+    <col min="30" max="30" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9.140625" style="10"/>
+    <col min="33" max="33" width="28.5703125" style="10" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="10"/>
+    <col min="35" max="35" width="23.5703125" style="11" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -850,10 +854,10 @@
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
@@ -882,71 +886,74 @@
         <v>29</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AD1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="23" t="s">
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AK1" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -992,9 +999,10 @@
       <c r="AR2"/>
       <c r="AS2"/>
       <c r="AT2"/>
+      <c r="AU2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ1">
+  <autoFilter ref="A1:AK1">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <sortState ref="A2:AG285">

</xml_diff>

<commit_message>
parse treatments from tagging data, #809
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AC$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,65 +24,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>DFO-MPO</author>
-  </authors>
-  <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DFO-MPO:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-yellow highlight indicates a later duplicate sample</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DFO-MPO:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-pp = precocious parr
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -156,9 +97,6 @@
     <t>duplicate</t>
   </si>
   <si>
-    <t>PIT tag</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
@@ -183,13 +121,7 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Precocity (1/0)</t>
-  </si>
-  <si>
     <t>surface water temp</t>
-  </si>
-  <si>
-    <t>Amt MS222(g)</t>
   </si>
   <si>
     <t>collection Date
@@ -197,6 +129,15 @@
   </si>
   <si>
     <t>life Stage</t>
+  </si>
+  <si>
+    <t>PIT Tag #</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -206,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,14 +159,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,26 +198,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -306,32 +219,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -362,66 +249,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,42 +647,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA10" sqref="AA10"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="9"/>
     <col min="3" max="3" width="20.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="9" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="9" customWidth="1"/>
-    <col min="11" max="12" width="4.42578125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.85546875" style="9" customWidth="1"/>
-    <col min="15" max="15" width="27.42578125" style="9" customWidth="1"/>
-    <col min="16" max="20" width="9.140625" style="9"/>
-    <col min="21" max="22" width="10.7109375" style="9" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" style="9" customWidth="1"/>
-    <col min="24" max="29" width="9.140625" style="9"/>
-    <col min="30" max="30" width="16.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="9.140625" style="9"/>
-    <col min="33" max="33" width="28.5703125" style="9" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" style="9"/>
-    <col min="35" max="35" width="23.5703125" style="10" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="9" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9" customWidth="1"/>
+    <col min="10" max="11" width="4.42578125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="27.42578125" style="9" customWidth="1"/>
+    <col min="15" max="19" width="9.140625" style="9"/>
+    <col min="20" max="21" width="10.7109375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" style="9" customWidth="1"/>
+    <col min="23" max="28" width="9.140625" style="9"/>
+    <col min="29" max="29" width="16.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -816,99 +685,91 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>21</v>
+      <c r="Q1" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="15" t="s">
+      <c r="U1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AB1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AC1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
-      <c r="D2"/>
+      <c r="D2" s="17"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
@@ -944,26 +805,13 @@
       <c r="AK2"/>
       <c r="AL2"/>
       <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK1">
-    <filterColumn colId="3" showButton="0"/>
-  </autoFilter>
+  <autoFilter ref="A1:AC1"/>
   <sortState ref="A2:AG285">
     <sortCondition ref="A2:A285"/>
   </sortState>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="J1">
+  <conditionalFormatting sqref="I1">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>
@@ -974,7 +822,7 @@
   <conditionalFormatting sqref="C1">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"'TRUE'"</formula>
     </cfRule>
@@ -988,6 +836,5 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix heritage recursion, add ufid cols to parsers, fix comments. #825
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
@@ -36,23 +36,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. STW</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>eg. STW</t>
         </r>
       </text>
     </comment>
@@ -60,23 +49,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. EQU
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">eg. EQU
 </t>
         </r>
       </text>
@@ -85,23 +63,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional,  can specify unit as either (cm) or (mm)</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional,  can specify unit as either (cm) or (mm)</t>
         </r>
       </text>
     </comment>
@@ -109,23 +76,25 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, can specify unit as either (g) or (kg)</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, can specify unit as either (g) or (kg)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, calculated in application.</t>
         </r>
       </text>
     </comment>
@@ -133,23 +102,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -157,23 +115,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -181,23 +128,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -205,23 +141,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -229,23 +154,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, precocity.  Should be a 1/0, Y/N value</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, precocity.  Should be a 1/0, Y/N value</t>
         </r>
       </text>
     </comment>
@@ -253,23 +167,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, eg. AB, CD</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, eg. AB, CD</t>
         </r>
       </text>
     </comment>
@@ -277,23 +180,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. 1999</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>eg. 1999</t>
         </r>
       </text>
     </comment>
@@ -301,23 +193,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. Jan</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>eg. Jan</t>
         </r>
       </text>
     </comment>
@@ -325,23 +206,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-eg 1</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>eg 1</t>
         </r>
       </text>
     </comment>
@@ -349,23 +219,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -373,23 +232,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -518,7 +366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,13 +418,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1035,10 +876,10 @@
   <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V5:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
utility function to select groups and containers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-pit tagging.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AC$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$AD$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -66,13 +66,26 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999 FP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t>Optional,  can specify unit as either (cm) or (mm)</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Fish #</t>
   </si>
@@ -358,6 +371,9 @@
   <si>
     <t>Amount</t>
   </si>
+  <si>
+    <t>Collection</t>
+  </si>
 </sst>
 </file>
 
@@ -366,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +438,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -873,13 +895,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="O6:P6"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,21 +910,21 @@
     <col min="3" max="3" width="20.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="9" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="9" customWidth="1"/>
-    <col min="10" max="11" width="4.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.85546875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" style="9" customWidth="1"/>
-    <col min="15" max="19" width="9.140625" style="9"/>
-    <col min="20" max="21" width="10.7109375" style="9" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="9" customWidth="1"/>
-    <col min="23" max="28" width="9.140625" style="9"/>
-    <col min="29" max="29" width="16.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="9"/>
+    <col min="6" max="7" width="11.140625" style="9" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="9" customWidth="1"/>
+    <col min="11" max="12" width="4.42578125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.85546875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" style="9" customWidth="1"/>
+    <col min="16" max="20" width="9.140625" style="9"/>
+    <col min="21" max="22" width="10.7109375" style="9" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="9" customWidth="1"/>
+    <col min="24" max="29" width="9.140625" style="9"/>
+    <col min="30" max="30" width="16.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -921,77 +943,80 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" s="17"/>
@@ -1030,13 +1055,14 @@
       <c r="AK2"/>
       <c r="AL2"/>
       <c r="AM2"/>
+      <c r="AN2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC1"/>
+  <autoFilter ref="A1:AD1"/>
   <sortState ref="A2:AG285">
     <sortCondition ref="A2:A285"/>
   </sortState>
-  <conditionalFormatting sqref="I1">
+  <conditionalFormatting sqref="J1">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0.8</formula>
     </cfRule>

</xml_diff>